<commit_message>
omer- set login and scroll
</commit_message>
<xml_diff>
--- a/pet proj.xlsx
+++ b/pet proj.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omer\Desktop\desktop\Projects-May-19\pet-treat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A65F0AB-6F54-4EE8-8B19-79B3DEFA2B1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD02B00-99A7-40AC-9A46-48CADF21A38D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="1395" windowWidth="14625" windowHeight="13440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="2085" windowWidth="14625" windowHeight="13440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>users</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>reviews</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>Front</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>_id</t>
   </si>
   <si>
@@ -299,6 +293,12 @@
   </si>
   <si>
     <t>fromUserId</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>dogId</t>
   </si>
 </sst>
 </file>
@@ -1090,17 +1090,17 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1114,7 @@
   <dimension ref="B1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1142,198 +1142,198 @@
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="6"/>
       <c r="G3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="6"/>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6"/>
       <c r="G5" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6"/>
       <c r="G6" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6"/>
       <c r="G7" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8"/>
       <c r="H8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
         <v>31</v>
-      </c>
-      <c r="I8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E9" s="6"/>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E10" s="6"/>
       <c r="H10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E11" s="8"/>
       <c r="G11" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E12" s="6"/>
       <c r="H12" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E13" s="6"/>
       <c r="H13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E14" s="6"/>
       <c r="H14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G17" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="7:9" x14ac:dyDescent="0.2">
       <c r="H18" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.2">
       <c r="H19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1365,7 +1365,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
@@ -1377,43 +1377,43 @@
     </row>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>63</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -1421,19 +1421,19 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -1441,19 +1441,19 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>71</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
@@ -1461,16 +1461,16 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="14"/>
@@ -1479,19 +1479,19 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>64</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>65</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1499,16 +1499,16 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="14"/>
@@ -1517,19 +1517,19 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1537,19 +1537,19 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="18"/>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="18"/>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="18"/>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="18"/>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="19"/>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="19"/>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="19"/>

</xml_diff>